<commit_message>
Add Morchella eximia to list of additions
</commit_message>
<xml_diff>
--- a/data/raw_data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/raw_data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Kenai_NWR_checklist\KenaiNWRspecies\data\taxonomy_additions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\Kenai_NWR_checklist\KenaiNWRspecies\data\raw_data\taxonomy_additions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="154">
   <si>
     <t>Scientific Name with Authority</t>
   </si>
@@ -536,6 +536,24 @@
   </si>
   <si>
     <t>https://www.gbif.org/species/9669747|https://www.mycobank.org/page/Name%20details%20page/name/Cytospora%20notastroma</t>
+  </si>
+  <si>
+    <t>Morchella eximia Boud.</t>
+  </si>
+  <si>
+    <t>Morchella eximia</t>
+  </si>
+  <si>
+    <t>excellent morel</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Morchella&lt;/em&gt; &lt;em&gt;eximia&lt;/em&gt; Boud.</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Morchella&lt;/em&gt; &lt;em&gt;eximia&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/7258337</t>
   </si>
 </sst>
 </file>
@@ -711,6 +729,16 @@
   <dxfs count="8">
     <dxf>
       <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -736,16 +764,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1293,11 +1311,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1533,6 +1551,38 @@
         <v>147</v>
       </c>
     </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="12">
+        <v>20</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="12">
+        <v>670397</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="duplicateValues" dxfId="7" priority="6"/>
@@ -1544,7 +1594,7 @@
     <cfRule type="duplicateValues" dxfId="5" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="5">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Scientific Name text" error="Scientific Name must be text between 2 and 87 characters in length." sqref="C1:C5 C7:C1048576">
@@ -1891,16 +1941,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="A6:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6 C1 C8:C1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D1 D9:D1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="5">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1 G6 G8:G1048576">
@@ -5524,6 +5574,44 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
+    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
+        </TermInfo>
+      </Terms>
+    </ka8aab2ab8224e0695cc7b5356d06aef>
+    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
+        </TermInfo>
+      </Terms>
+    </j9add0d2db884c689b68553fead24975>
+    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
+    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Value>934</Value>
+      <Value>395</Value>
+    </TaxCatchAll>
+    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
+    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
+    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
+      <Description>HDAZSPZUFV6T-1059-12</Description>
+    </_dlc_DocIdUrl>
+    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -5569,45 +5657,16 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
-    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
-        </TermInfo>
-      </Terms>
-    </ka8aab2ab8224e0695cc7b5356d06aef>
-    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
-        </TermInfo>
-      </Terms>
-    </j9add0d2db884c689b68553fead24975>
-    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
-    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Value>934</Value>
-      <Value>395</Value>
-    </TaxCatchAll>
-    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
-    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
-    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
-      <Description>HDAZSPZUFV6T-1059-12</Description>
-    </_dlc_DocIdUrl>
-    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Other Content" ma:contentTypeID="0x0101000369F4E336BE6248A5FAEDCEB8DA0DAE061300945D0A02AE6B6B4CB6A222311EE2147A" ma:contentTypeVersion="10" ma:contentTypeDescription="Catch all bucket for everything else not fitting under another content type for the project. " ma:contentTypeScope="" ma:versionID="3a543d46be299152b17bb026b54c55fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0c7fc5b747229e76245c7ff85f8b9e1" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5825,24 +5884,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
@@ -5859,7 +5901,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45A28C5D-483C-4E1D-84EE-E79440036366}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5876,12 +5934,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Morchella pulchella to the additions list
</commit_message>
<xml_diff>
--- a/data/raw_data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/raw_data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="160">
   <si>
     <t>Scientific Name with Authority</t>
   </si>
@@ -554,6 +554,24 @@
   </si>
   <si>
     <t>https://www.gbif.org/species/7258337</t>
+  </si>
+  <si>
+    <t>Morchella pulchella Clowez &amp; Franç.Petit</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Morchella&lt;/em&gt; &lt;em&gt;pulchella&lt;/em&gt; Clowez &amp; Franç.Petit</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Morchella&lt;/em&gt; &lt;em&gt;pulchella&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/7665238</t>
+  </si>
+  <si>
+    <t>pretty morel</t>
+  </si>
+  <si>
+    <t>Morchella pulchella</t>
   </si>
 </sst>
 </file>
@@ -1311,11 +1329,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1581,6 +1599,38 @@
       </c>
       <c r="M8" s="12" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="12">
+        <v>21</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="12">
+        <v>670397</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -5574,44 +5624,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
-    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
-        </TermInfo>
-      </Terms>
-    </ka8aab2ab8224e0695cc7b5356d06aef>
-    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
-        </TermInfo>
-      </Terms>
-    </j9add0d2db884c689b68553fead24975>
-    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
-    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Value>934</Value>
-      <Value>395</Value>
-    </TaxCatchAll>
-    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
-    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
-    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
-      <Description>HDAZSPZUFV6T-1059-12</Description>
-    </_dlc_DocIdUrl>
-    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -5657,16 +5669,45 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
+    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
+        </TermInfo>
+      </Terms>
+    </ka8aab2ab8224e0695cc7b5356d06aef>
+    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
+        </TermInfo>
+      </Terms>
+    </j9add0d2db884c689b68553fead24975>
+    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
+    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Value>934</Value>
+      <Value>395</Value>
+    </TaxCatchAll>
+    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
+    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
+    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
+      <Description>HDAZSPZUFV6T-1059-12</Description>
+    </_dlc_DocIdUrl>
+    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Other Content" ma:contentTypeID="0x0101000369F4E336BE6248A5FAEDCEB8DA0DAE061300945D0A02AE6B6B4CB6A222311EE2147A" ma:contentTypeVersion="10" ma:contentTypeDescription="Catch all bucket for everything else not fitting under another content type for the project. " ma:contentTypeScope="" ma:versionID="3a543d46be299152b17bb026b54c55fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0c7fc5b747229e76245c7ff85f8b9e1" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5884,7 +5925,24 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
@@ -5901,23 +5959,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45A28C5D-483C-4E1D-84EE-E79440036366}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5934,4 +5976,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Morchella sextelata to the additions list
</commit_message>
<xml_diff>
--- a/data/raw_data/taxonomy_additions/FWSpecies_additions.xlsx
+++ b/data/raw_data/taxonomy_additions/FWSpecies_additions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="166">
   <si>
     <t>Scientific Name with Authority</t>
   </si>
@@ -572,6 +572,24 @@
   </si>
   <si>
     <t>Morchella pulchella</t>
+  </si>
+  <si>
+    <t>Morchella sextelata M.Kuo</t>
+  </si>
+  <si>
+    <t>sixth morel</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Morchella&lt;/em&gt; &lt;em&gt;sextelata&lt;/em&gt; M.Kuo</t>
+  </si>
+  <si>
+    <t>https://www.gbif.org/species/7561838</t>
+  </si>
+  <si>
+    <t>&lt;em&gt;Morchella&lt;/em&gt; &lt;em&gt;sextelata&lt;/em&gt;</t>
+  </si>
+  <si>
+    <t>Morchella sextelata</t>
   </si>
 </sst>
 </file>
@@ -744,7 +762,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sheet1" xfId="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1329,11 +1357,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1633,25 +1661,60 @@
         <v>157</v>
       </c>
     </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="12">
+        <v>22</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="12">
+        <v>670397</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C5 C7:C1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="12"/>
+  <conditionalFormatting sqref="C1:C5 C7:C9 C11:C1048576">
+    <cfRule type="duplicateValues" dxfId="6" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Scientific Name text" error="Scientific Name must be text between 2 and 87 characters in length." sqref="C1:C5 C7:C1048576">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Scientific Name text" error="Scientific Name must be text between 2 and 87 characters in length." sqref="C1:C5 C7:C9 C11:C1048576">
       <formula1>2</formula1>
       <formula2>87</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sci. Name w/auth. text" error="Scientific Name with Authority must be text between 3 and 175 characters in length." sqref="D1:D1048576 C6">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sci. Name w/auth. text" error="Scientific Name with Authority must be text between 3 and 175 characters in length." sqref="D1:D1048576 C6 C10">
       <formula1>3</formula1>
       <formula2>175</formula2>
     </dataValidation>
@@ -1991,16 +2054,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="A6:A1048576 A1">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6 C1 C8:C1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6 D1 D9:D1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="5">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1 G6 G8:G1048576">
@@ -5624,6 +5687,44 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
+    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
+        </TermInfo>
+      </Terms>
+    </ka8aab2ab8224e0695cc7b5356d06aef>
+    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
+        </TermInfo>
+      </Terms>
+    </j9add0d2db884c689b68553fead24975>
+    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
+    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Value>934</Value>
+      <Value>395</Value>
+    </TaxCatchAll>
+    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
+    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
+    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
+      <Description>HDAZSPZUFV6T-1059-12</Description>
+    </_dlc_DocIdUrl>
+    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -5669,45 +5770,16 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FinalDel xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</FinalDel>
-    <ka8aab2ab8224e0695cc7b5356d06aef xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">IMD</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">a91fd69b-97f8-4ca9-9612-2465a56690c0</TermId>
-        </TermInfo>
-      </Terms>
-    </ka8aab2ab8224e0695cc7b5356d06aef>
-    <j9add0d2db884c689b68553fead24975 xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Taxonomy</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">142b6aa6-14af-44d5-a482-c1af7b57b297</TermId>
-        </TermInfo>
-      </Terms>
-    </j9add0d2db884c689b68553fead24975>
-    <_dlc_DocId xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">HDAZSPZUFV6T-1059-12</_dlc_DocId>
-    <TaxCatchAll xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Value>934</Value>
-      <Value>395</Value>
-    </TaxCatchAll>
-    <ArchContent xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">false</ArchContent>
-    <KpiDescription xmlns="http://schemas.microsoft.com/sharepoint/v3">Draft Electronic Data Deliverable (EDD) for batch load of taxon records to Taxonomy.</KpiDescription>
-    <_dlc_DocIdUrl xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Url>https://nrss.sharepoint.nps.gov/div/imd/co/irma/_layouts/DocIdRedir.aspx?ID=HDAZSPZUFV6T-1059-12</Url>
-      <Description>HDAZSPZUFV6T-1059-12</Description>
-    </_dlc_DocIdUrl>
-    <TaxKeywordTaxHTField xmlns="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Other Content" ma:contentTypeID="0x0101000369F4E336BE6248A5FAEDCEB8DA0DAE061300945D0A02AE6B6B4CB6A222311EE2147A" ma:contentTypeVersion="10" ma:contentTypeDescription="Catch all bucket for everything else not fitting under another content type for the project. " ma:contentTypeScope="" ma:versionID="3a543d46be299152b17bb026b54c55fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a0c7fc5b747229e76245c7ff85f8b9e1" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5925,24 +5997,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D834B1-5D0B-462D-A423-7D3D4ABAD784}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="2f7f3c08-2512-4e1c-9e4b-e5327eed3f75"/>
@@ -5959,7 +6014,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEAF0FC-C686-46B5-BD8F-92FE129ED9A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45A28C5D-483C-4E1D-84EE-E79440036366}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5976,12 +6047,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B796EF64-841D-4FA0-9A82-9CBF4A2112C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>